<commit_message>
code added till checkout
</commit_message>
<xml_diff>
--- a/src/main/java/com/primeclass/qa/testdata/PrimeclassData.xlsx
+++ b/src/main/java/com/primeclass/qa/testdata/PrimeclassData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\010645_puresoft\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CEF538F-35A1-4D4E-B93F-4E2EC4227B7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13673C6A-1ED7-4DB1-80C4-DF64C929EC1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B58FED1-E6F3-4CCE-966B-CB97FC14D8F0}"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" r:id="rId1"/>
-    <sheet name="ParentSignUp" sheetId="7" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId2"/>
+    <sheet name="ParentSignUp" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="47">
   <si>
     <t>Firstname</t>
   </si>
@@ -73,10 +74,106 @@
     <t>Vipul Saxena</t>
   </si>
   <si>
-    <t>0000000222</t>
-  </si>
-  <si>
-    <t>0000000333</t>
+    <t>Exam courses - No row should insert in STG and PSwd table</t>
+  </si>
+  <si>
+    <t>Regular courses-Offline--and Online both</t>
+  </si>
+  <si>
+    <t>IC006-offline and online both</t>
+  </si>
+  <si>
+    <t>For online journey only entry should be made into Ps_Aes_Stdnt_Pswd.</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>ONLINE Journey</t>
+  </si>
+  <si>
+    <t>Dw005, and Reg</t>
+  </si>
+  <si>
+    <t>check for</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Lastname</t>
+  </si>
+  <si>
+    <t>Parent name</t>
+  </si>
+  <si>
+    <t>parent mobile</t>
+  </si>
+  <si>
+    <t>streetAddress</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>pin code</t>
+  </si>
+  <si>
+    <t>Shiping_state</t>
+  </si>
+  <si>
+    <t>Arun</t>
+  </si>
+  <si>
+    <t>Pandey</t>
+  </si>
+  <si>
+    <t>Ak Pandey</t>
+  </si>
+  <si>
+    <t>9560370108</t>
+  </si>
+  <si>
+    <t>arunpandey.pus@aesl.in</t>
+  </si>
+  <si>
+    <t>JKHouse- Plot 32 Pusa road</t>
+  </si>
+  <si>
+    <t>Noida</t>
+  </si>
+  <si>
+    <t>201305</t>
+  </si>
+  <si>
+    <t>Uttar Pradesh</t>
+  </si>
+  <si>
+    <t>1000000222</t>
+  </si>
+  <si>
+    <t>arunpandey1@yopmail.com</t>
+  </si>
+  <si>
+    <t>vipul1231@yopmail.com</t>
+  </si>
+  <si>
+    <t>2000000333</t>
+  </si>
+  <si>
+    <t>classes</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>- Any -</t>
   </si>
 </sst>
 </file>
@@ -148,7 +245,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -156,6 +253,20 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -471,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6473CB0D-1CBA-4422-BE1A-F0DE286CDFB4}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -484,10 +595,19 @@
     <col min="4" max="4" width="23.7265625" style="1" customWidth="1"/>
     <col min="5" max="5" width="22.90625" style="1" customWidth="1"/>
     <col min="6" max="6" width="11.36328125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="1"/>
+    <col min="7" max="7" width="8.7265625" style="1"/>
+    <col min="8" max="8" width="14.08984375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.26953125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.54296875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="20.36328125" style="1" customWidth="1"/>
+    <col min="12" max="13" width="15" style="1" customWidth="1"/>
+    <col min="14" max="14" width="15.90625" style="1" customWidth="1"/>
+    <col min="15" max="16" width="8.7265625" style="1"/>
+    <col min="17" max="17" width="15.36328125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -506,19 +626,52 @@
       <c r="F1" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="G1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>8</v>
@@ -526,38 +679,169 @@
       <c r="F2" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="G2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>8</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{5E63A2B8-4D1A-4CF9-8B50-B56F16F23A09}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{906FB6CF-1EA6-4832-B1B1-891738DC8E01}"/>
+    <hyperlink ref="K2" r:id="rId3" xr:uid="{B7B9497A-6820-4B86-A9F2-B1048F342598}"/>
+    <hyperlink ref="K3" r:id="rId4" xr:uid="{C5A3B8D7-21C0-413B-8CB9-8A719EA8381F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5B1D6E1-EBEB-41F7-A737-553651E98D00}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="70.36328125" customWidth="1"/>
+    <col min="2" max="2" width="62.81640625" customWidth="1"/>
+    <col min="3" max="3" width="14.08984375" customWidth="1"/>
+    <col min="4" max="4" width="20.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:B3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E5A258-7319-4193-8C59-A04F716F499C}">
   <dimension ref="A1:F3"/>
   <sheetViews>

</xml_diff>

<commit_message>
Minre code added for calender
</commit_message>
<xml_diff>
--- a/src/main/java/com/primeclass/qa/testdata/PrimeclassData.xlsx
+++ b/src/main/java/com/primeclass/qa/testdata/PrimeclassData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\010645_puresoft\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13673C6A-1ED7-4DB1-80C4-DF64C929EC1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44864319-2F96-461C-9E99-24FC8E318B1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B58FED1-E6F3-4CCE-966B-CB97FC14D8F0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
   <si>
     <t>Firstname</t>
   </si>
@@ -149,31 +149,22 @@
     <t>Uttar Pradesh</t>
   </si>
   <si>
-    <t>1000000222</t>
-  </si>
-  <si>
-    <t>arunpandey1@yopmail.com</t>
-  </si>
-  <si>
-    <t>vipul1231@yopmail.com</t>
-  </si>
-  <si>
-    <t>2000000333</t>
-  </si>
-  <si>
     <t>classes</t>
   </si>
   <si>
     <t>state</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>12</t>
   </si>
   <si>
     <t>- Any -</t>
+  </si>
+  <si>
+    <t>11500000222</t>
+  </si>
+  <si>
+    <t>arunpandey14@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -257,15 +248,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -582,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6473CB0D-1CBA-4422-BE1A-F0DE286CDFB4}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -627,25 +618,25 @@
         <v>9</v>
       </c>
       <c r="G1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="J1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>1</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>43</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>25</v>
@@ -665,13 +656,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>8</v>
@@ -679,26 +670,26 @@
       <c r="F2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>46</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>34</v>
@@ -710,71 +701,16 @@
         <v>36</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q3" s="5" t="s">
         <v>37</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{5E63A2B8-4D1A-4CF9-8B50-B56F16F23A09}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{906FB6CF-1EA6-4832-B1B1-891738DC8E01}"/>
-    <hyperlink ref="K2" r:id="rId3" xr:uid="{B7B9497A-6820-4B86-A9F2-B1048F342598}"/>
-    <hyperlink ref="K3" r:id="rId4" xr:uid="{C5A3B8D7-21C0-413B-8CB9-8A719EA8381F}"/>
+    <hyperlink ref="M2" r:id="rId2" xr:uid="{B7B9497A-6820-4B86-A9F2-B1048F342598}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -798,7 +734,7 @@
       <c r="A1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C1" s="7"/>
@@ -807,14 +743,14 @@
       <c r="A2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="9"/>
+      <c r="B2" s="12"/>
       <c r="C2" s="7"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="9"/>
+      <c r="B3" s="12"/>
       <c r="C3" s="7" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
code added till purchase journey
</commit_message>
<xml_diff>
--- a/src/main/java/com/primeclass/qa/testdata/PrimeclassData.xlsx
+++ b/src/main/java/com/primeclass/qa/testdata/PrimeclassData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\010645_puresoft\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44864319-2F96-461C-9E99-24FC8E318B1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9EF9E4C-3FC9-4660-9464-1C934D222C5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B58FED1-E6F3-4CCE-966B-CB97FC14D8F0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
   <si>
     <t>Firstname</t>
   </si>
@@ -158,13 +158,19 @@
     <t>12</t>
   </si>
   <si>
-    <t>- Any -</t>
-  </si>
-  <si>
-    <t>11500000222</t>
-  </si>
-  <si>
-    <t>arunpandey14@yopmail.com</t>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>center</t>
+  </si>
+  <si>
+    <t>Delhi - Pitampura (Engineering)</t>
+  </si>
+  <si>
+    <t>11800000222</t>
+  </si>
+  <si>
+    <t>arunpandey17@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -573,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6473CB0D-1CBA-4422-BE1A-F0DE286CDFB4}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -588,17 +594,18 @@
     <col min="6" max="6" width="11.36328125" style="1" customWidth="1"/>
     <col min="7" max="7" width="8.7265625" style="1"/>
     <col min="8" max="8" width="14.08984375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.26953125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.54296875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="20.36328125" style="1" customWidth="1"/>
-    <col min="12" max="13" width="15" style="1" customWidth="1"/>
-    <col min="14" max="14" width="15.90625" style="1" customWidth="1"/>
-    <col min="15" max="16" width="8.7265625" style="1"/>
-    <col min="17" max="17" width="15.36328125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.7265625" style="1"/>
+    <col min="9" max="9" width="19.81640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.26953125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.54296875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="20.36328125" style="1" customWidth="1"/>
+    <col min="13" max="14" width="15" style="1" customWidth="1"/>
+    <col min="15" max="15" width="15.90625" style="1" customWidth="1"/>
+    <col min="16" max="17" width="8.7265625" style="1"/>
+    <col min="18" max="18" width="15.36328125" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -623,46 +630,49 @@
       <c r="H1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>8</v>
@@ -676,38 +686,41 @@
       <c r="H2" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="Q2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="R2" s="5" t="s">
         <v>37</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{5E63A2B8-4D1A-4CF9-8B50-B56F16F23A09}"/>
-    <hyperlink ref="M2" r:id="rId2" xr:uid="{B7B9497A-6820-4B86-A9F2-B1048F342598}"/>
+    <hyperlink ref="N2" r:id="rId2" xr:uid="{B7B9497A-6820-4B86-A9F2-B1048F342598}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>

</xml_diff>